<commit_message>
Update figures and data for PyIRoGlass paper
</commit_message>
<xml_diff>
--- a/Epsilon_Inversion/EpsilonRegression.xlsx
+++ b/Epsilon_Inversion/EpsilonRegression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahshi/Documents/GitHub/PyIRoGlass/Epsilon_Inversion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4695F1DF-C0D0-4A45-8B55-EF000BB74DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE461C43-FDE2-794A-9B2F-FD8A833475CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="31920" windowHeight="20380" activeTab="3" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="31920" windowHeight="20380" activeTab="3" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
   </bookViews>
   <sheets>
     <sheet name="NIRRegress" sheetId="4" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1415,12 +1415,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7739,8 +7733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D56AC5-DAA9-8140-A576-6658D6B454A7}">
   <dimension ref="A1:BW36"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15330,8 +15324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F3C50D-B1DF-E247-95AB-3AD4B1033E27}">
   <dimension ref="A1:BY36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8:T8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15611,7 +15605,7 @@
         <v>148</v>
       </c>
       <c r="AB2" s="15"/>
-      <c r="AC2" s="117"/>
+      <c r="AC2" s="16"/>
       <c r="AD2" s="18"/>
       <c r="AE2" s="16">
         <v>265</v>
@@ -15714,7 +15708,7 @@
       <c r="AB3" s="15">
         <v>284</v>
       </c>
-      <c r="AC3" s="117">
+      <c r="AC3" s="16">
         <v>5</v>
       </c>
       <c r="AD3" s="18"/>
@@ -15889,7 +15883,7 @@
       <c r="AB4" s="15">
         <v>207</v>
       </c>
-      <c r="AC4" s="117">
+      <c r="AC4" s="16">
         <v>22</v>
       </c>
       <c r="AD4" s="18"/>
@@ -16064,7 +16058,7 @@
       <c r="AB5" s="15">
         <v>375</v>
       </c>
-      <c r="AC5" s="117">
+      <c r="AC5" s="16">
         <v>20</v>
       </c>
       <c r="AD5" s="18"/>
@@ -16277,7 +16271,7 @@
       <c r="AB6" s="15">
         <v>180</v>
       </c>
-      <c r="AC6" s="117">
+      <c r="AC6" s="16">
         <v>15</v>
       </c>
       <c r="AD6" s="18"/>
@@ -16455,7 +16449,7 @@
       <c r="AB7" s="15">
         <v>398</v>
       </c>
-      <c r="AC7" s="117">
+      <c r="AC7" s="16">
         <v>10</v>
       </c>
       <c r="AD7" s="18"/>
@@ -16633,7 +16627,7 @@
       <c r="AB8" s="15">
         <v>303.435</v>
       </c>
-      <c r="AC8" s="117">
+      <c r="AC8" s="16">
         <v>9.1959999999999997</v>
       </c>
       <c r="AD8" s="18"/>
@@ -16847,7 +16841,7 @@
       <c r="AB9" s="15">
         <v>361</v>
       </c>
-      <c r="AC9" s="117">
+      <c r="AC9" s="16">
         <v>43</v>
       </c>
       <c r="AD9" s="18"/>
@@ -17026,7 +17020,7 @@
       <c r="AB10" s="15">
         <v>349</v>
       </c>
-      <c r="AC10" s="117">
+      <c r="AC10" s="16">
         <v>25</v>
       </c>
       <c r="AD10" s="18"/>
@@ -17204,7 +17198,7 @@
       <c r="AB11" s="15">
         <v>380</v>
       </c>
-      <c r="AC11" s="117">
+      <c r="AC11" s="16">
         <v>30</v>
       </c>
       <c r="AD11" s="18"/>
@@ -17378,7 +17372,7 @@
       <c r="AB12" s="15">
         <v>372</v>
       </c>
-      <c r="AC12" s="117">
+      <c r="AC12" s="16">
         <v>14</v>
       </c>
       <c r="AD12" s="18"/>
@@ -17552,7 +17546,7 @@
       <c r="AB13" s="15">
         <v>394</v>
       </c>
-      <c r="AC13" s="117">
+      <c r="AC13" s="16">
         <v>27</v>
       </c>
       <c r="AD13" s="18"/>
@@ -17726,7 +17720,7 @@
       <c r="AB14" s="15">
         <v>385</v>
       </c>
-      <c r="AC14" s="117">
+      <c r="AC14" s="16">
         <v>18</v>
       </c>
       <c r="AD14" s="18"/>
@@ -17900,7 +17894,7 @@
       <c r="AB15" s="15">
         <v>359</v>
       </c>
-      <c r="AC15" s="117">
+      <c r="AC15" s="16">
         <v>25</v>
       </c>
       <c r="AD15" s="18"/>
@@ -18074,7 +18068,7 @@
       <c r="AB16" s="15">
         <v>355</v>
       </c>
-      <c r="AC16" s="117"/>
+      <c r="AC16" s="16"/>
       <c r="AD16" s="18"/>
       <c r="AE16" s="16">
         <v>355</v>
@@ -18252,7 +18246,7 @@
         <v>148</v>
       </c>
       <c r="AB17" s="15"/>
-      <c r="AC17" s="117"/>
+      <c r="AC17" s="16"/>
       <c r="AD17" s="18"/>
       <c r="AE17" s="16">
         <v>356</v>
@@ -18418,7 +18412,7 @@
         <v>148</v>
       </c>
       <c r="AB18" s="15"/>
-      <c r="AC18" s="117"/>
+      <c r="AC18" s="16"/>
       <c r="AD18" s="18"/>
       <c r="AE18" s="16">
         <v>264</v>
@@ -18587,7 +18581,7 @@
         <v>148</v>
       </c>
       <c r="AB19" s="15"/>
-      <c r="AC19" s="117"/>
+      <c r="AC19" s="16"/>
       <c r="AD19" s="18"/>
       <c r="AE19" s="16">
         <v>244</v>
@@ -18756,7 +18750,7 @@
         <v>148</v>
       </c>
       <c r="AB20" s="15"/>
-      <c r="AC20" s="117"/>
+      <c r="AC20" s="16"/>
       <c r="AD20" s="18"/>
       <c r="AE20" s="16">
         <v>294</v>
@@ -19108,7 +19102,7 @@
       <c r="AB22" s="94">
         <v>308</v>
       </c>
-      <c r="AC22" s="118">
+      <c r="AC22" s="13">
         <v>110</v>
       </c>
       <c r="AD22" s="35"/>
@@ -19279,7 +19273,7 @@
       <c r="AB23" s="15">
         <v>284</v>
       </c>
-      <c r="AC23" s="117">
+      <c r="AC23" s="16">
         <v>5</v>
       </c>
       <c r="AD23" s="18"/>
@@ -19454,7 +19448,7 @@
       <c r="AB24" s="15">
         <v>207</v>
       </c>
-      <c r="AC24" s="117">
+      <c r="AC24" s="16">
         <v>22</v>
       </c>
       <c r="AD24" s="18"/>
@@ -19629,7 +19623,7 @@
       <c r="AB25" s="15">
         <v>375</v>
       </c>
-      <c r="AC25" s="117">
+      <c r="AC25" s="16">
         <v>20</v>
       </c>
       <c r="AD25" s="18"/>
@@ -19752,7 +19746,7 @@
       <c r="AB26" s="15">
         <v>180</v>
       </c>
-      <c r="AC26" s="117">
+      <c r="AC26" s="16">
         <v>15</v>
       </c>
       <c r="AD26" s="18"/>
@@ -19930,7 +19924,7 @@
       <c r="AB27" s="15">
         <v>398</v>
       </c>
-      <c r="AC27" s="117">
+      <c r="AC27" s="16">
         <v>10</v>
       </c>
       <c r="AD27" s="18"/>
@@ -20108,7 +20102,7 @@
       <c r="AB28" s="15">
         <v>303.435</v>
       </c>
-      <c r="AC28" s="117">
+      <c r="AC28" s="16">
         <v>9.1959999999999997</v>
       </c>
       <c r="AD28" s="18"/>
@@ -20322,7 +20316,7 @@
       <c r="AB29" s="15">
         <v>361</v>
       </c>
-      <c r="AC29" s="117">
+      <c r="AC29" s="16">
         <v>43</v>
       </c>
       <c r="AD29" s="18"/>
@@ -20501,7 +20495,7 @@
       <c r="AB30" s="15">
         <v>349</v>
       </c>
-      <c r="AC30" s="117">
+      <c r="AC30" s="16">
         <v>25</v>
       </c>
       <c r="AD30" s="18"/>
@@ -20679,7 +20673,7 @@
       <c r="AB31" s="15">
         <v>380</v>
       </c>
-      <c r="AC31" s="117">
+      <c r="AC31" s="16">
         <v>30</v>
       </c>
       <c r="AD31" s="18"/>
@@ -20853,7 +20847,7 @@
       <c r="AB32" s="15">
         <v>372</v>
       </c>
-      <c r="AC32" s="117">
+      <c r="AC32" s="16">
         <v>14</v>
       </c>
       <c r="AD32" s="18"/>
@@ -21027,7 +21021,7 @@
       <c r="AB33" s="15">
         <v>394</v>
       </c>
-      <c r="AC33" s="117">
+      <c r="AC33" s="16">
         <v>27</v>
       </c>
       <c r="AD33" s="18"/>
@@ -21201,7 +21195,7 @@
       <c r="AB34" s="15">
         <v>385</v>
       </c>
-      <c r="AC34" s="117">
+      <c r="AC34" s="16">
         <v>18</v>
       </c>
       <c r="AD34" s="18"/>
@@ -21375,7 +21369,7 @@
       <c r="AB35" s="15">
         <v>359</v>
       </c>
-      <c r="AC35" s="117">
+      <c r="AC35" s="16">
         <v>25</v>
       </c>
       <c r="AD35" s="18"/>

</xml_diff>